<commit_message>
feat: Proteger rutas de historial y eliminar test-import
</commit_message>
<xml_diff>
--- a/doc/excel pruebas/presupuesto.xlsx
+++ b/doc/excel pruebas/presupuesto.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="76">
   <si>
     <t>Fecha</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>A0000300001345</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -246,7 +252,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;S&quot;000"/>
     <numFmt numFmtId="165" formatCode="&quot;V&quot;000"/>
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -390,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,9 +436,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -459,9 +462,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -485,7 +485,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -806,7 +806,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -830,213 +830,213 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.6">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="R1" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="T1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="U1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="V1" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="W1" s="32" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="36">
+      <c r="F2" s="34">
         <v>45068</v>
       </c>
-      <c r="G2" s="37">
+      <c r="G2" s="35">
         <v>1</v>
       </c>
-      <c r="H2" s="38">
+      <c r="H2" s="36">
         <v>0</v>
       </c>
-      <c r="I2" s="38">
+      <c r="I2" s="36">
         <v>1</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="38">
+      <c r="K2" s="36">
         <v>860056.89</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="P2" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="Q2" s="35" t="s">
+      <c r="Q2" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="R2" s="38">
+      <c r="R2" s="36">
         <v>78.37</v>
       </c>
-      <c r="S2" s="38">
+      <c r="S2" s="36">
         <v>9069.68</v>
       </c>
-      <c r="T2" s="38">
+      <c r="T2" s="36">
         <v>710790.82</v>
       </c>
-      <c r="U2" s="35" t="s">
+      <c r="U2" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="V2" s="38">
+      <c r="V2" s="36">
         <v>0</v>
       </c>
-      <c r="W2" s="36"/>
+      <c r="W2" s="34"/>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="34">
         <v>45314</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="35">
         <v>1</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="36">
         <v>0</v>
       </c>
-      <c r="I3" s="38">
+      <c r="I3" s="36">
         <v>1</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="38">
+      <c r="K3" s="36">
         <v>1525667.12</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="35" t="s">
+      <c r="M3" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="35" t="s">
+      <c r="N3" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="O3" s="35" t="s">
+      <c r="O3" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="P3" s="35" t="s">
+      <c r="P3" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="Q3" s="35" t="s">
+      <c r="Q3" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="R3" s="38">
+      <c r="R3" s="36">
         <v>21.63</v>
       </c>
-      <c r="S3" s="38">
+      <c r="S3" s="36">
         <v>58293.2</v>
       </c>
-      <c r="T3" s="38">
+      <c r="T3" s="36">
         <v>1260881.9199999999</v>
       </c>
-      <c r="U3" s="35" t="s">
+      <c r="U3" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="V3" s="38">
+      <c r="V3" s="36">
         <v>0</v>
       </c>
-      <c r="W3" s="36"/>
+      <c r="W3" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1113,7 +1113,7 @@
       <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="37" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1133,25 +1133,35 @@
       <c r="E2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="17">
+      <c r="F2" s="13">
+        <v>45012</v>
+      </c>
+      <c r="G2" s="13">
+        <v>45717</v>
+      </c>
+      <c r="H2" s="15">
+        <v>100</v>
+      </c>
+      <c r="I2" s="13">
+        <v>45717</v>
+      </c>
+      <c r="J2" s="16">
         <f>3896.78</f>
         <v>3896.78</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20" t="s">
+      <c r="M2" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="21">
+      <c r="O2" s="20">
         <v>1</v>
       </c>
       <c r="P2" s="12">
@@ -1163,40 +1173,50 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="22">
+      <c r="A3" s="21">
         <v>406</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <v>45176</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="27">
+      <c r="F3" s="23">
+        <v>45176</v>
+      </c>
+      <c r="G3" s="13">
+        <v>45718</v>
+      </c>
+      <c r="H3" s="15">
+        <v>100</v>
+      </c>
+      <c r="I3" s="13">
+        <v>45718</v>
+      </c>
+      <c r="J3" s="25">
         <f>944.72</f>
         <v>944.72</v>
       </c>
-      <c r="K3" s="28" t="s">
+      <c r="K3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="29" t="s">
+      <c r="L3" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30">
+      <c r="M3" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="28">
         <v>1409</v>
       </c>
-      <c r="O3" s="31">
+      <c r="O3" s="29">
         <v>1</v>
       </c>
       <c r="P3" s="12">
@@ -1208,38 +1228,50 @@
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="22">
+      <c r="A4" s="21">
         <v>412</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>45229</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="27">
+      <c r="F4" s="23">
+        <v>45229</v>
+      </c>
+      <c r="G4" s="13">
+        <v>45719</v>
+      </c>
+      <c r="H4" s="15">
+        <v>100</v>
+      </c>
+      <c r="I4" s="13">
+        <v>45719</v>
+      </c>
+      <c r="J4" s="25">
         <f>1925*2</f>
         <v>3850</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="31">
+      <c r="M4" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" s="28">
+        <v>1409</v>
+      </c>
+      <c r="O4" s="29">
         <v>1</v>
       </c>
       <c r="P4" s="12">
@@ -1251,40 +1283,50 @@
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>417</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>45243</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27">
+      <c r="F5" s="23">
+        <v>45243</v>
+      </c>
+      <c r="G5" s="13">
+        <v>45720</v>
+      </c>
+      <c r="H5" s="15">
+        <v>100</v>
+      </c>
+      <c r="I5" s="13">
+        <v>45720</v>
+      </c>
+      <c r="J5" s="25">
         <f>4020</f>
         <v>4020</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="29" t="s">
+      <c r="L5" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30" t="s">
+      <c r="M5" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="31">
+      <c r="O5" s="29">
         <v>1</v>
       </c>
       <c r="P5" s="12">
@@ -1296,39 +1338,49 @@
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>419</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <v>45271</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27">
+      <c r="F6" s="23">
+        <v>45271</v>
+      </c>
+      <c r="G6" s="13">
+        <v>45721</v>
+      </c>
+      <c r="H6" s="15">
+        <v>100</v>
+      </c>
+      <c r="I6" s="13">
+        <v>45721</v>
+      </c>
+      <c r="J6" s="25">
         <v>1682</v>
       </c>
-      <c r="K6" s="28" t="s">
+      <c r="K6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="29" t="s">
+      <c r="L6" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30">
+      <c r="M6" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" s="28">
         <v>1324</v>
       </c>
-      <c r="O6" s="31">
+      <c r="O6" s="29">
         <v>1</v>
       </c>
       <c r="P6" s="12">
@@ -1340,40 +1392,50 @@
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="32">
+      <c r="A7" s="30">
         <v>2989</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="31">
         <v>44918</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="23">
+      <c r="F7" s="31">
+        <v>44918</v>
+      </c>
+      <c r="G7" s="13">
+        <v>45722</v>
+      </c>
+      <c r="H7" s="15">
+        <v>100</v>
+      </c>
+      <c r="I7" s="13">
+        <v>45722</v>
+      </c>
+      <c r="J7" s="22">
         <f>4065869</f>
         <v>4065869</v>
       </c>
-      <c r="K7" s="28" t="s">
+      <c r="K7" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="29" t="s">
+      <c r="L7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30" t="s">
+      <c r="M7" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="31">
+      <c r="O7" s="29">
         <v>1</v>
       </c>
       <c r="P7" s="12">
@@ -1385,40 +1447,50 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="32">
+      <c r="A8" s="30">
         <v>2989</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="31">
         <v>44918</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="23">
+      <c r="F8" s="31">
+        <v>44918</v>
+      </c>
+      <c r="G8" s="13">
+        <v>45723</v>
+      </c>
+      <c r="H8" s="15">
+        <v>100</v>
+      </c>
+      <c r="I8" s="13">
+        <v>45723</v>
+      </c>
+      <c r="J8" s="22">
         <f>26138</f>
         <v>26138</v>
       </c>
-      <c r="K8" s="28" t="s">
+      <c r="K8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="29" t="s">
+      <c r="L8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30" t="s">
+      <c r="M8" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N8" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="O8" s="31">
+      <c r="O8" s="29">
         <v>1</v>
       </c>
       <c r="P8" s="12">
@@ -1431,7 +1503,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:I2 I3:I8">
+  <conditionalFormatting sqref="H2">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>